<commit_message>
changed get_match_data to get_active_match_data. built notes around data analysis requirements
</commit_message>
<xml_diff>
--- a/Deadlock_Player_Hero_Data/test_match_data.xlsx
+++ b/Deadlock_Player_Hero_Data/test_match_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77419a36fcbd9f93/Documents/Local Code/Deadlock Database/Deadlock_Player_Hero_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_778170B7D3C05D510B993411595ED87656CCDC23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{014B8D4E-9BC9-4179-AD2C-33A94FB89F7A}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_778170B7D3C05D510B993411595ED87656CCDC23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C51D864F-C395-4A69-B2B8-FC48EC49548D}"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="1860" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41625" yWindow="4005" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,6 +131,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,15 +424,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>